<commit_message>
XL SAVE File With BarChart Done
</commit_message>
<xml_diff>
--- a/xl/save.xlsx
+++ b/xl/save.xlsx
@@ -64,10 +64,10 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -86,49 +86,6 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr/>
-          <a:p>
-            <a:r>
-              <a:t/>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-      <overlay val="0"/>
-      <spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-      <txPr>
-        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" baseline="0" i="0" kern="1200" spc="0" strike="noStrike" sz="1400">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </txPr>
-    </title>
     <plotArea>
       <layout/>
       <barChart>
@@ -138,218 +95,12 @@
         <ser>
           <idx val="0"/>
           <order val="0"/>
-          <tx>
-            <strRef>
-              <f>Sheet1!$C$1</f>
-              <strCache>
-                <ptCount val="1"/>
-                <pt idx="0">
-                  <v>price</v>
-                </pt>
-              </strCache>
-            </strRef>
-          </tx>
           <spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
             <a:ln>
-              <a:noFill/>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <invertIfNegative val="0"/>
-          <cat>
-            <multiLvlStrRef>
-              <multiLvlStrCache>
-                <lvl>
-                  <pt idx="0">
-                    <v>1</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>2</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>3</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>4</v>
-                  </pt>
-                </lvl>
-                <lvl>
-                  <pt idx="0">
-                    <v>1001</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>1002</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>1003</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>1004</v>
-                  </pt>
-                </lvl>
-              </multiLvlStrCache>
-              <f>Sheet1!$A$2:$B$5</f>
-            </multiLvlStrRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>Sheet1!$C$2:$C$5</f>
-              <numCache>
-                <formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</formatCode>
-                <ptCount val="4"/>
-                <pt idx="0">
-                  <v>5.95</v>
-                </pt>
-                <pt idx="1">
-                  <v>6.96</v>
-                </pt>
-                <pt idx="2">
-                  <v>7.95</v>
-                </pt>
-                <pt idx="3">
-                  <v>8.67</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="1"/>
-          <order val="1"/>
-          <tx>
-            <strRef>
-              <f>Sheet1!$D$1</f>
-              <strCache>
-                <ptCount val="1"/>
-              </strCache>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <invertIfNegative val="0"/>
-          <cat>
-            <multiLvlStrRef>
-              <multiLvlStrCache>
-                <lvl>
-                  <pt idx="0">
-                    <v>1</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>2</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>3</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>4</v>
-                  </pt>
-                </lvl>
-                <lvl>
-                  <pt idx="0">
-                    <v>1001</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>1002</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>1003</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>1004</v>
-                  </pt>
-                </lvl>
-              </multiLvlStrCache>
-              <f>Sheet1!$A$2:$B$5</f>
-            </multiLvlStrRef>
-          </cat>
-          <val>
-            <numRef>
-              <f>Sheet1!$D$2:$D$5</f>
-              <numCache>
-                <formatCode>General</formatCode>
-                <ptCount val="4"/>
-                <pt idx="0">
-                  <v>5.355</v>
-                </pt>
-                <pt idx="1">
-                  <v>6.255</v>
-                </pt>
-                <pt idx="2">
-                  <v>7.155</v>
-                </pt>
-                <pt idx="3">
-                  <v>7.801</v>
-                </pt>
-              </numCache>
-            </numRef>
-          </val>
-        </ser>
-        <ser>
-          <idx val="2"/>
-          <order val="2"/>
-          <tx>
-            <strRef>
-              <f>Sheet1!$E$1</f>
-              <strCache>
-                <ptCount val="1"/>
-              </strCache>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <invertIfNegative val="0"/>
-          <cat>
-            <multiLvlStrRef>
-              <multiLvlStrCache>
-                <lvl>
-                  <pt idx="0">
-                    <v>1</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>2</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>3</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>4</v>
-                  </pt>
-                </lvl>
-                <lvl>
-                  <pt idx="0">
-                    <v>1001</v>
-                  </pt>
-                  <pt idx="1">
-                    <v>1002</v>
-                  </pt>
-                  <pt idx="2">
-                    <v>1003</v>
-                  </pt>
-                  <pt idx="3">
-                    <v>1004</v>
-                  </pt>
-                </lvl>
-              </multiLvlStrCache>
-              <f>Sheet1!$A$2:$B$5</f>
-            </multiLvlStrRef>
-          </cat>
           <val>
             <numRef>
               <f>Sheet1!$E$2:$E$5</f>
@@ -380,170 +131,104 @@
           <showPercent val="0"/>
           <showBubbleSize val="0"/>
         </dLbls>
-        <gapWidth val="219"/>
-        <overlap val="-27"/>
-        <axId val="495374432"/>
-        <axId val="495375744"/>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
       </barChart>
       <catAx>
-        <axId val="495374432"/>
+        <axId val="10"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
         <delete val="0"/>
         <axPos val="b"/>
-        <numFmt formatCode="General" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:noFill/>
-          <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:prstDash val="solid"/>
-            <a:round/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </txPr>
-        <crossAx val="495375744"/>
+        <crossAx val="100"/>
         <crosses val="autoZero"/>
-        <auto val="1"/>
+        <auto val="0"/>
         <lblAlgn val="ctr"/>
         <lblOffset val="100"/>
         <noMultiLvlLbl val="0"/>
       </catAx>
       <valAx>
-        <axId val="495375744"/>
+        <axId val="100"/>
         <scaling>
           <orientation val="minMax"/>
         </scaling>
         <delete val="0"/>
         <axPos val="l"/>
-        <majorGridlines>
-          <spPr>
-            <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-              <a:round/>
-            </a:ln>
-          </spPr>
-        </majorGridlines>
+        <majorGridlines/>
         <numFmt formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)" sourceLinked="1"/>
         <majorTickMark val="none"/>
         <minorTickMark val="none"/>
         <tickLblPos val="nextTo"/>
-        <spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-          </a:ln>
-        </spPr>
-        <txPr>
-          <a:bodyPr anchor="ctr" anchorCtr="1" rot="-60000000" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:t/>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </txPr>
-        <crossAx val="495374432"/>
+        <crossAx val="10"/>
         <crosses val="autoZero"/>
         <crossBetween val="between"/>
       </valAx>
     </plotArea>
     <legend>
-      <legendPos val="b"/>
-      <layout>
-        <manualLayout>
-          <xMode val="edge"/>
-          <yMode val="edge"/>
-          <wMode val="factor"/>
-          <hMode val="factor"/>
-          <x val="0.3424227909011374"/>
-          <y val="0.894096675415573"/>
-          <w val="0.3651544181977253"/>
-          <h val="0.07812554680664917"/>
-        </manualLayout>
-      </layout>
+      <legendPos val="r"/>
       <overlay val="0"/>
-      <spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </spPr>
-      <txPr>
-        <a:bodyPr anchor="ctr" anchorCtr="1" rot="0" spcFirstLastPara="1" vert="horz" vertOverflow="ellipsis" wrap="square"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr b="0" baseline="0" i="0" kern="1200" strike="noStrike" sz="900">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:r>
-            <a:t/>
-          </a:r>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </txPr>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <chart>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <val>
+            <numRef>
+              <f>'Sheet1'!$D$2:$D$5</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
     </legend>
     <plotVisOnly val="1"/>
     <dispBlanksAs val="gap"/>
@@ -553,19 +238,14 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <twoCellAnchor>
+  <oneCellAnchor>
     <from>
-      <col>6</col>
-      <colOff>0</colOff>
-      <row>5</row>
+      <col>5</col>
+      <colOff>590550</colOff>
+      <row>1</row>
       <rowOff>9525</rowOff>
     </from>
-    <to>
-      <col>13</col>
-      <colOff>304800</colOff>
-      <row>19</row>
-      <rowOff>85725</rowOff>
-    </to>
+    <ext cx="5400000" cy="2700000"/>
     <graphicFrame>
       <nvGraphicFramePr>
         <cNvPr id="1" name="Chart 1"/>
@@ -579,7 +259,29 @@
       </a:graphic>
     </graphicFrame>
     <clientData/>
-  </twoCellAnchor>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>5</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="2" name="Chart 2"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
 </wsDr>
 </file>
 
@@ -853,7 +555,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -864,12 +566,12 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>transaction_id</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>product_id</t>
         </is>
@@ -879,20 +581,20 @@
           <t>price</t>
         </is>
       </c>
-      <c r="D1" s="2" t="n"/>
-      <c r="E1" s="2" t="n"/>
+      <c r="D1" s="1" t="n"/>
+      <c r="E1" s="1" t="n"/>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="n">
+      <c r="A2" s="1" t="n">
         <v>1001</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="5" t="n">
         <v>5.95</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="1" t="n">
         <v>5.355</v>
       </c>
       <c r="E2" s="5">
@@ -901,16 +603,16 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="1" t="n">
         <v>1002</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="5" t="n">
         <v>6.96</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="1" t="n">
         <v>6.264</v>
       </c>
       <c r="E3" s="5">
@@ -919,16 +621,16 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="1" t="n">
         <v>1003</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="5" t="n">
         <v>7.95</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="1" t="n">
         <v>7.155</v>
       </c>
       <c r="E4" s="5">
@@ -937,16 +639,16 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="n">
+      <c r="A5" s="1" t="n">
         <v>1004</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="1" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="5" t="n">
         <v>8.67</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="1" t="n">
         <v>7.803</v>
       </c>
       <c r="E5" s="5">

</xml_diff>